<commit_message>
Após alterar os diretórios das pastas o funcionamento via android foi prejudicado, ele não executa da forma correta e fecha o programa, fora isso no computador está tudo certo
</commit_message>
<xml_diff>
--- a/app/data/db_calc_rdmarcas.xlsx
+++ b/app/data/db_calc_rdmarcas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,14 +446,46 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B2" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>4000</v>
+      </c>
+      <c r="B3" t="n">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4000</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4740</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4041</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
-          <t>5000.0</t>
+          <t>4141.0</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
-          <t>5000.0</t>
+          <t>4142.0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Foi ajustado alguns avisos no código, não interfere no funcionamento geral
</commit_message>
<xml_diff>
--- a/app/data/db_calc_rdmarcas.xlsx
+++ b/app/data/db_calc_rdmarcas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,10 +447,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5000</v>
+        <v>5001</v>
       </c>
       <c r="B2" t="n">
-        <v>5000</v>
+        <v>5050</v>
       </c>
     </row>
     <row r="3">
@@ -486,15 +486,19 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>4000.0</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>4000.0</t>
-        </is>
+      <c r="A7" t="n">
+        <v>4000</v>
+      </c>
+      <c r="B7" t="n">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8000</v>
+      </c>
+      <c r="B8" t="n">
+        <v>8000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionando informações na lista RD-Marcas
</commit_message>
<xml_diff>
--- a/app/data/db_calc_rdmarcas.xlsx
+++ b/app/data/db_calc_rdmarcas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +445,62 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>4512.4</v>
+      </c>
+      <c r="B2" t="n">
+        <v>5012.4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5475.3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>8451.200000000001</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>8800</v>
+      </c>
+      <c r="B4" t="n">
+        <v>8900</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>9000</v>
+      </c>
+      <c r="B5" t="n">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>9000.6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>15060.1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>4800</v>
+      </c>
+      <c r="B7" t="n">
+        <v>9220</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7000</v>
+      </c>
+      <c r="B8" t="n">
+        <v>4650.08</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Foi implementado os sons ao clicar nos botões dos popups
</commit_message>
<xml_diff>
--- a/app/data/db_calc_rdmarcas.xlsx
+++ b/app/data/db_calc_rdmarcas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,62 +445,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>4512.4</v>
-      </c>
-      <c r="B2" t="n">
-        <v>5012.4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>5475.3</v>
-      </c>
-      <c r="B3" t="n">
-        <v>8451.200000000001</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>8800</v>
-      </c>
-      <c r="B4" t="n">
-        <v>8900</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>9000</v>
-      </c>
-      <c r="B5" t="n">
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>9000.6</v>
-      </c>
-      <c r="B6" t="n">
-        <v>15060.1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>4800</v>
-      </c>
-      <c r="B7" t="n">
-        <v>9220</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7000</v>
-      </c>
-      <c r="B8" t="n">
-        <v>4650.08</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>